<commit_message>
done with result windows probably
</commit_message>
<xml_diff>
--- a/ProjectSportyStuff/test.xlsx
+++ b/ProjectSportyStuff/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,39 @@
   </si>
   <si>
     <t>eargrae</t>
+  </si>
+  <si>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t>fefe</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>kokokaka</t>
+  </si>
+  <si>
+    <t>jahny</t>
+  </si>
+  <si>
+    <t>hayayay</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>womansson</t>
+  </si>
+  <si>
+    <t>smithy</t>
+  </si>
+  <si>
+    <t>barack</t>
+  </si>
+  <si>
+    <t>obama</t>
   </si>
 </sst>
 </file>
@@ -129,7 +162,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -295,6 +328,38 @@
         <v>1233.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>995.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1233.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -302,7 +367,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -349,6 +414,211 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>771.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>895.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support for auto fill of text fields after login.
</commit_message>
<xml_diff>
--- a/ProjectSportyStuff/test.xlsx
+++ b/ProjectSportyStuff/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kam\git\Testdesign tekniker och exekvering av test\ProjectSportyStuff\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majanorrman/git/ProjectSportyStuff/ProjectSportyStuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6D01D-66B2-494B-8127-259E9F22A946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A5704-B7BF-0F43-9E11-E30D83015383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1840" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Women" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -166,10 +166,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,8 +202,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,13 +521,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -562,9 +570,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5.0</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -572,10 +580,31 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>7.0</v>
+      <c r="D3">
+        <v>10.5</v>
+      </c>
+      <c r="E3">
+        <v>110.5</v>
+      </c>
+      <c r="F3">
+        <v>20.5</v>
+      </c>
+      <c r="G3">
+        <v>10.3</v>
+      </c>
+      <c r="H3">
+        <v>10.25</v>
+      </c>
+      <c r="I3">
+        <v>155.5</v>
+      </c>
+      <c r="J3">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -584,9 +613,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>8.0</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -595,9 +624,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>12.0</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -606,9 +635,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>15.0</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -626,13 +655,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,7 +713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -695,9 +724,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4.0</v>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -706,9 +735,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>6.0</v>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -717,9 +746,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>9.0</v>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -728,9 +757,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>10.0</v>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -738,10 +767,40 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>11.0</v>
+      <c r="D7">
+        <v>9.5</v>
+      </c>
+      <c r="E7">
+        <v>15.6</v>
+      </c>
+      <c r="F7">
+        <v>100.21</v>
+      </c>
+      <c r="G7" s="1">
+        <v>110.5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>150.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>10.25</v>
+      </c>
+      <c r="K7" s="1">
+        <v>10.55</v>
+      </c>
+      <c r="L7" s="1">
+        <v>10.525</v>
+      </c>
+      <c r="M7" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
@@ -750,9 +809,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>13.0</v>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -761,9 +820,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>14.0</v>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
@@ -772,9 +831,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>16.0</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
new commit a bit of changes
</commit_message>
<xml_diff>
--- a/ProjectSportyStuff/test.xlsx
+++ b/ProjectSportyStuff/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>ighkj</t>
+  </si>
+  <si>
+    <t>uhoujä</t>
+  </si>
+  <si>
+    <t>höjhk</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -609,6 +615,17 @@
       </c>
       <c r="C7" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made program reopen login/signup on exit
</commit_message>
<xml_diff>
--- a/ProjectSportyStuff/test.xlsx
+++ b/ProjectSportyStuff/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,51 @@
   </si>
   <si>
     <t>jenny</t>
+  </si>
+  <si>
+    <t>donald</t>
+  </si>
+  <si>
+    <t>trump</t>
+  </si>
+  <si>
+    <t>hillary</t>
+  </si>
+  <si>
+    <t>clinton</t>
+  </si>
+  <si>
+    <t>barack</t>
+  </si>
+  <si>
+    <t>obama</t>
+  </si>
+  <si>
+    <t>michelle</t>
+  </si>
+  <si>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t>haha</t>
+  </si>
+  <si>
+    <t>heaher</t>
+  </si>
+  <si>
+    <t>earhaer</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>htrrt</t>
+  </si>
+  <si>
+    <t>etha</t>
+  </si>
+  <si>
+    <t>rtahr</t>
   </si>
 </sst>
 </file>
@@ -114,7 +159,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -184,6 +229,134 @@
         <v>1233.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>995.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1233.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>995.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1233.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>995.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1233.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>995.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1233.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -191,7 +364,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -279,6 +452,170 @@
         <v>264.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="n">
+        <v>929.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>461.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>901.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>825.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>972.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>264.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>